<commit_message>
Adición de datos Fitoplancton
</commit_message>
<xml_diff>
--- a/01_Analisis_Exploratorio/02_Datos/Biologicos/DarwinCore/ListadoControlado.xlsx
+++ b/01_Analisis_Exploratorio/02_Datos/Biologicos/DarwinCore/ListadoControlado.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Expedicion_Pacifico\2021\Ictioplancton\Analisis_Exp_Pac\Ictioplancton_ExPacifico2021\01_Analisis_Exploratorio\02_Datos\Biologicos\DarwinCore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Ictioplancton_ExPacifico2021\01_Analisis_Exploratorio\02_Datos\Biologicos\DarwinCore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F024C53E-988D-4E85-89F7-91E0C78DC358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{8E6A034F-35B5-477F-86AC-7772F3D212D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="833" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="S06B" sheetId="1" r:id="rId1"/>
-    <sheet name="S06A" sheetId="2" r:id="rId2"/>
-    <sheet name="S05A" sheetId="3" r:id="rId3"/>
-    <sheet name="S05B" sheetId="4" r:id="rId4"/>
+    <sheet name="S05B" sheetId="4" r:id="rId2"/>
+    <sheet name="S06A" sheetId="2" r:id="rId3"/>
+    <sheet name="S05A" sheetId="3" r:id="rId4"/>
     <sheet name="S04A" sheetId="5" r:id="rId5"/>
-    <sheet name="S04B" sheetId="6" r:id="rId6"/>
+    <sheet name="S03A" sheetId="7" r:id="rId6"/>
+    <sheet name="S04B" sheetId="6" r:id="rId7"/>
+    <sheet name="S03B" sheetId="8" r:id="rId8"/>
+    <sheet name="G06A" sheetId="9" r:id="rId9"/>
+    <sheet name="Hoja5" sheetId="11" r:id="rId10"/>
+    <sheet name="G05A" sheetId="10" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="5" r:id="rId12"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="188">
   <si>
     <t>Bacteriastrum hyalinum</t>
   </si>
@@ -481,12 +488,135 @@
   </si>
   <si>
     <t>Rhizopsolenia imbricata</t>
+  </si>
+  <si>
+    <t>Ceratocoris horrida</t>
+  </si>
+  <si>
+    <t>Chaetoceros brevis complex</t>
+  </si>
+  <si>
+    <t>Cianobacteria</t>
+  </si>
+  <si>
+    <t>aff Dactiliosolen</t>
+  </si>
+  <si>
+    <t>aff Surriliella</t>
+  </si>
+  <si>
+    <t>Protoperidinium circular</t>
+  </si>
+  <si>
+    <t>Lithodesmiun undulatum</t>
+  </si>
+  <si>
+    <t>Phalacroma rapa</t>
+  </si>
+  <si>
+    <t>Ditylum brigthwelli</t>
+  </si>
+  <si>
+    <t>Protoperidinium pentagonal-falconiforma</t>
+  </si>
+  <si>
+    <t>Coscinodicus sp 2</t>
+  </si>
+  <si>
+    <t>Coscinodiscus waillessii</t>
+  </si>
+  <si>
+    <t>Cerataulina dentata</t>
+  </si>
+  <si>
+    <t>Ditylum brigthwellii</t>
+  </si>
+  <si>
+    <t>Rhizolenia imbricata</t>
+  </si>
+  <si>
+    <t>Neocallitera robusta</t>
+  </si>
+  <si>
+    <t>Rhizolenia imbricata var. Shrubsolei</t>
+  </si>
+  <si>
+    <t>Protoperidinium sp 1</t>
+  </si>
+  <si>
+    <t>Tripos macroceros</t>
+  </si>
+  <si>
+    <t>Stephanopixys turris</t>
+  </si>
+  <si>
+    <t>Guinardia delicatula</t>
+  </si>
+  <si>
+    <t>Entomoneis sp</t>
+  </si>
+  <si>
+    <t>Thalassiosira sp</t>
+  </si>
+  <si>
+    <t>Actinocyclus senarius</t>
+  </si>
+  <si>
+    <t>litodesmium undulatum</t>
+  </si>
+  <si>
+    <t>Cerataulina ?</t>
+  </si>
+  <si>
+    <t>Tripos fusus</t>
+  </si>
+  <si>
+    <t>Nepcalliptrella robusta</t>
+  </si>
+  <si>
+    <t>Gunardia delicatula</t>
+  </si>
+  <si>
+    <t>Prortoperidinium (pentagonal)</t>
+  </si>
+  <si>
+    <t>Ditylium</t>
+  </si>
+  <si>
+    <t>chaetoceros danicus</t>
+  </si>
+  <si>
+    <t>Ceratocory horrida</t>
+  </si>
+  <si>
+    <t>Dinoflagelados 1</t>
+  </si>
+  <si>
+    <t>tripos massiliensis</t>
+  </si>
+  <si>
+    <t>Central desconocida</t>
+  </si>
+  <si>
+    <t>Hemiaulus membranaceus</t>
+  </si>
+  <si>
+    <t>Tripos candelabrus</t>
+  </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t>(en blanco)</t>
+  </si>
+  <si>
+    <t>Total general</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -529,7 +659,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -537,10 +667,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="1" xr:uid="{0CF90D18-5A03-4286-B3CC-2855E3DC53D7}"/>
+    <cellStyle name="Normal 4" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -553,6 +687,641 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Christian Bermúdez-Rivas" refreshedDate="44830.727491898149" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="88">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B2:C64" sheet="G05A"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="Trieres chinensis" numFmtId="0">
+      <sharedItems containsBlank="1" count="40">
+        <s v="Lioloma elongatum"/>
+        <s v="Odontella aurita"/>
+        <s v="Chaetoceros diversus"/>
+        <s v="Bacteriastrum delicatulum"/>
+        <s v="Thalassionema nitzschioides"/>
+        <m/>
+        <s v="Coscinodiscus gigas"/>
+        <s v="Coscinodiscus sp 2"/>
+        <s v="Lithodesmium undulatum"/>
+        <s v="Trieres mobiliensis"/>
+        <s v="Coscinodiscus perforatus"/>
+        <s v="Coscinodiscus granii"/>
+        <s v="Skeletonema constatum"/>
+        <s v="Prortoperidinium (pentagonal)"/>
+        <s v="Tripos fusus"/>
+        <s v="Rhizosolenia setigera"/>
+        <s v="Coscinodiscus radiatus"/>
+        <s v="Gyrosigma sp"/>
+        <s v="Coscinodiscus sp "/>
+        <s v="Chaetoceros affinis"/>
+        <s v="Nitzschia sp"/>
+        <s v="Cerataulina pelagica"/>
+        <s v="Ditylium"/>
+        <s v="Hobaniella longicruris"/>
+        <s v="chaetoceros danicus"/>
+        <s v="Podolampas bipes"/>
+        <s v="Coscinodiscopsis jonesiana"/>
+        <s v="Guinardia flaccida"/>
+        <s v="Phalacroma rapa"/>
+        <s v="Ceratocory horrida"/>
+        <s v="Trieres chinensis"/>
+        <s v="Dinoflagelados 1"/>
+        <s v="Navicula sp"/>
+        <s v="Cerataulina dentata"/>
+        <s v="tripos massiliensis"/>
+        <s v="Tripos muelleri"/>
+        <s v="Central desconocida"/>
+        <s v="Hemiaulus membranaceus"/>
+        <s v="Tripos candelabrus"/>
+        <s v="Bacteriastrum hyalinum"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="1" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="26" count="10">
+        <n v="1"/>
+        <n v="4"/>
+        <n v="2"/>
+        <n v="3"/>
+        <m/>
+        <n v="5"/>
+        <n v="10"/>
+        <n v="6"/>
+        <n v="26"/>
+        <n v="7"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="88">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="32"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="33"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="34"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="35"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="36"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="37"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="38"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="39"/>
+    <x v="9"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:A44" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="41">
+        <item x="3"/>
+        <item x="39"/>
+        <item x="36"/>
+        <item x="33"/>
+        <item x="21"/>
+        <item x="29"/>
+        <item x="19"/>
+        <item x="24"/>
+        <item x="2"/>
+        <item x="26"/>
+        <item x="6"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="31"/>
+        <item x="22"/>
+        <item x="27"/>
+        <item x="17"/>
+        <item x="37"/>
+        <item x="23"/>
+        <item x="0"/>
+        <item x="8"/>
+        <item x="32"/>
+        <item x="20"/>
+        <item x="1"/>
+        <item x="28"/>
+        <item x="25"/>
+        <item x="13"/>
+        <item x="15"/>
+        <item x="12"/>
+        <item x="4"/>
+        <item x="30"/>
+        <item x="9"/>
+        <item x="38"/>
+        <item x="14"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="41">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -851,10 +1620,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20B2502-5791-4AEE-96E8-E5A4D83B02A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1234,15 +2003,1161 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A45">
+  <sortState ref="A2:A45">
     <sortCondition ref="A2:A45"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:A44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>183</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>176</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>42</v>
+      </c>
+      <c r="C60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>184</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>173</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>181</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B2:C64">
+    <sortCondition ref="B2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98272D93-D2C2-4E9F-BE0D-D87648C188B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <f>SUM(B1:B46)</f>
+        <v>1107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1705,18 +3620,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B94">
+  <sortState ref="A1:B94">
     <sortCondition ref="A1:A94"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57DCFC1-3889-4D0F-AD71-D990D56F52B2}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2103,407 +4018,15 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B46">
+  <sortState ref="A1:B46">
     <sortCondition ref="A1:A46"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DDB718-0D92-40EF-8575-618B96BD91D6}">
-  <dimension ref="A1:B47"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>115</v>
-      </c>
-      <c r="B14">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>108</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>113</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>112</v>
-      </c>
-      <c r="B19">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>107</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>109</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>114</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>119</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>110</v>
-      </c>
-      <c r="B33">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>120</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>123</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>117</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>122</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>118</v>
-      </c>
-      <c r="B46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <f>SUM(B1:B46)</f>
-        <v>1107</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F80C48-EE95-4693-A27E-48C10A230B90}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B44"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -2858,7 +4381,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B43">
+  <sortState ref="A2:B43">
     <sortCondition ref="A2:A43"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2866,10 +4389,223 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553123FA-5B69-478E-A019-F6C51EC5608E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B25"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:B37">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -3109,9 +4845,643 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B29">
+  <sortState ref="A2:B29">
     <sortCondition ref="A2:A29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B45"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>171</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>162</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>161</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>169</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>165</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:B88">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B31"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:B60">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adición de nuevos analisis
</commit_message>
<xml_diff>
--- a/01_Analisis_Exploratorio/02_Datos/Biologicos/DarwinCore/ListadoControlado.xlsx
+++ b/01_Analisis_Exploratorio/02_Datos/Biologicos/DarwinCore/ListadoControlado.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15375" windowHeight="7740" tabRatio="833" firstSheet="15" activeTab="35"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15375" windowHeight="7740" tabRatio="833" firstSheet="15" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="S06B" sheetId="1" r:id="rId1"/>
@@ -51,42 +51,42 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="30" r:id="rId37"/>
-    <pivotCache cacheId="31" r:id="rId38"/>
-    <pivotCache cacheId="32" r:id="rId39"/>
-    <pivotCache cacheId="33" r:id="rId40"/>
-    <pivotCache cacheId="34" r:id="rId41"/>
-    <pivotCache cacheId="35" r:id="rId42"/>
-    <pivotCache cacheId="36" r:id="rId43"/>
-    <pivotCache cacheId="37" r:id="rId44"/>
-    <pivotCache cacheId="38" r:id="rId45"/>
-    <pivotCache cacheId="39" r:id="rId46"/>
-    <pivotCache cacheId="40" r:id="rId47"/>
-    <pivotCache cacheId="41" r:id="rId48"/>
-    <pivotCache cacheId="42" r:id="rId49"/>
-    <pivotCache cacheId="43" r:id="rId50"/>
-    <pivotCache cacheId="44" r:id="rId51"/>
-    <pivotCache cacheId="45" r:id="rId52"/>
-    <pivotCache cacheId="46" r:id="rId53"/>
-    <pivotCache cacheId="47" r:id="rId54"/>
-    <pivotCache cacheId="48" r:id="rId55"/>
-    <pivotCache cacheId="49" r:id="rId56"/>
-    <pivotCache cacheId="50" r:id="rId57"/>
-    <pivotCache cacheId="51" r:id="rId58"/>
-    <pivotCache cacheId="52" r:id="rId59"/>
-    <pivotCache cacheId="53" r:id="rId60"/>
-    <pivotCache cacheId="54" r:id="rId61"/>
-    <pivotCache cacheId="55" r:id="rId62"/>
-    <pivotCache cacheId="56" r:id="rId63"/>
-    <pivotCache cacheId="57" r:id="rId64"/>
-    <pivotCache cacheId="60" r:id="rId65"/>
-    <pivotCache cacheId="63" r:id="rId66"/>
-    <pivotCache cacheId="66" r:id="rId67"/>
-    <pivotCache cacheId="69" r:id="rId68"/>
-    <pivotCache cacheId="72" r:id="rId69"/>
-    <pivotCache cacheId="75" r:id="rId70"/>
-    <pivotCache cacheId="78" r:id="rId71"/>
-    <pivotCache cacheId="81" r:id="rId72"/>
+    <pivotCache cacheId="157" r:id="rId37"/>
+    <pivotCache cacheId="158" r:id="rId38"/>
+    <pivotCache cacheId="159" r:id="rId39"/>
+    <pivotCache cacheId="160" r:id="rId40"/>
+    <pivotCache cacheId="161" r:id="rId41"/>
+    <pivotCache cacheId="162" r:id="rId42"/>
+    <pivotCache cacheId="163" r:id="rId43"/>
+    <pivotCache cacheId="164" r:id="rId44"/>
+    <pivotCache cacheId="165" r:id="rId45"/>
+    <pivotCache cacheId="166" r:id="rId46"/>
+    <pivotCache cacheId="167" r:id="rId47"/>
+    <pivotCache cacheId="168" r:id="rId48"/>
+    <pivotCache cacheId="169" r:id="rId49"/>
+    <pivotCache cacheId="170" r:id="rId50"/>
+    <pivotCache cacheId="171" r:id="rId51"/>
+    <pivotCache cacheId="172" r:id="rId52"/>
+    <pivotCache cacheId="173" r:id="rId53"/>
+    <pivotCache cacheId="174" r:id="rId54"/>
+    <pivotCache cacheId="175" r:id="rId55"/>
+    <pivotCache cacheId="176" r:id="rId56"/>
+    <pivotCache cacheId="177" r:id="rId57"/>
+    <pivotCache cacheId="178" r:id="rId58"/>
+    <pivotCache cacheId="179" r:id="rId59"/>
+    <pivotCache cacheId="180" r:id="rId60"/>
+    <pivotCache cacheId="181" r:id="rId61"/>
+    <pivotCache cacheId="182" r:id="rId62"/>
+    <pivotCache cacheId="183" r:id="rId63"/>
+    <pivotCache cacheId="184" r:id="rId64"/>
+    <pivotCache cacheId="185" r:id="rId65"/>
+    <pivotCache cacheId="186" r:id="rId66"/>
+    <pivotCache cacheId="187" r:id="rId67"/>
+    <pivotCache cacheId="188" r:id="rId68"/>
+    <pivotCache cacheId="189" r:id="rId69"/>
+    <pivotCache cacheId="190" r:id="rId70"/>
+    <pivotCache cacheId="191" r:id="rId71"/>
+    <pivotCache cacheId="192" r:id="rId72"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -8449,7 +8449,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica10" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica10" cacheId="183" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E46" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -8659,7 +8659,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica8" cacheId="81" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica8" cacheId="192" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -8849,7 +8849,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica10" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica10" cacheId="158" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -8995,7 +8995,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica8" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica8" cacheId="157" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -9077,7 +9077,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica11" cacheId="32" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica11" cacheId="159" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -9215,7 +9215,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica12" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica12" cacheId="160" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E40" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -9401,7 +9401,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica13" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica13" cacheId="161" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -9483,7 +9483,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica14" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica14" cacheId="162" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -9621,7 +9621,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica15" cacheId="36" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica15" cacheId="163" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -9739,7 +9739,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica16" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica16" cacheId="164" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -9857,7 +9857,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica17" cacheId="38" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica17" cacheId="165" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E36" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -10027,7 +10027,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica11" cacheId="57" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica11" cacheId="184" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -10245,7 +10245,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica18" cacheId="39" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica18" cacheId="166" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -10375,7 +10375,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica19" cacheId="40" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica19" cacheId="167" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E31" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -10525,7 +10525,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica20" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica20" cacheId="168" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -10619,7 +10619,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica21" cacheId="42" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica21" cacheId="169" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -10685,7 +10685,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica22" cacheId="43" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica22" cacheId="170" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -10771,7 +10771,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica23" cacheId="44" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica23" cacheId="171" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -10877,7 +10877,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica24" cacheId="45" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica24" cacheId="172" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -10999,7 +10999,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica25" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica25" cacheId="173" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -11141,7 +11141,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="47" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="174" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -11283,7 +11283,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="48" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="175" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -11365,7 +11365,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="60" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="185" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E57" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -11619,7 +11619,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica3" cacheId="49" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica3" cacheId="176" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -11729,7 +11729,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica4" cacheId="50" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica4" cacheId="177" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -11835,7 +11835,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="178" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -11945,7 +11945,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica6" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica6" cacheId="179" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -12059,7 +12059,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable34.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica7" cacheId="53" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica7" cacheId="180" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -12149,7 +12149,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable35.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica8" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica8" cacheId="181" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -12283,7 +12283,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable36.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica9" cacheId="55" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica9" cacheId="182" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E40" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -12469,7 +12469,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="63" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="186" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -12687,7 +12687,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica3" cacheId="66" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica3" cacheId="187" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E44" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -12889,7 +12889,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica4" cacheId="69" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica4" cacheId="188" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -13019,7 +13019,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="72" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -13165,7 +13165,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica6" cacheId="75" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica6" cacheId="190" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E46" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -13375,7 +13375,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica7" cacheId="78" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica7" cacheId="191" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -19553,7 +19553,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E47"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21942,8 +21942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26464,7 +26464,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27738,7 +27738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E39"/>
     </sheetView>
   </sheetViews>
@@ -28553,7 +28553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E47"/>
     </sheetView>
   </sheetViews>

</xml_diff>